<commit_message>
Added review for the coding phase
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Desktop\AN3\VVSS\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927F7BB4-C684-42AB-BB68-A296C1F6CECF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15585AB5-2A3A-4C15-9CC1-48391785DE50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -194,6 +194,54 @@
   </si>
   <si>
     <t>Mag Raul</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>OrdersGUIController / 88, 92
+KitchenGUIController / 55, 64</t>
+  </si>
+  <si>
+    <t>Formatul de afisare al orei este gresit in cazul in care minutele sunt mai mici de 10 (ex: 13:05 va fi afisat 13:5)</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>OrdersGUIController / 141
+KitchenGUIContorller / 53, 61</t>
+  </si>
+  <si>
+    <t>Aplicatia permite apasarea unor butoane fara a selecta un element dintr-o lista in situatii in care ar fi necesar acest lucru. Astfel apar erori netratate</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>MainGUIController
+KitchenGUIContorller</t>
+  </si>
+  <si>
+    <t>Nu se asteapta inchiderea tuturor meselor inainte de inchiderea bucatariei, respectiv inchiderea bucatariei inainte de inchiderea restaurantului</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>MenuDataModel / 12</t>
+  </si>
+  <si>
+    <t>Numele parametrilor constructorului creeaza confuzie</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>KitchenGUIController / 29</t>
+  </si>
+  <si>
+    <t>Bucla while continua executia pana la inchiderea aplicatiei, chiar daca fereastra aferenta bucatariei a fost inchisa mai devreme</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1172,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,8 +1491,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,9 +1500,10 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="4" max="4" width="28.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="55.140625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="11.28515625" style="6" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
@@ -1489,8 +1538,12 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="18">
+        <v>234</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
@@ -1503,8 +1556,12 @@
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="3">
+        <v>234</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
@@ -1549,49 +1606,79 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -1745,7 +1832,9 @@
         <v>8</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>1.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated Architectural Design Defects review form
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Desktop\AN3\VVSS\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Documents\GitHub\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15585AB5-2A3A-4C15-9CC1-48391785DE50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57921BCC-2942-43DD-99BA-BEF5C4199EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Bucla while continua executia pana la inchiderea aplicatiei, chiar daca fereastra aferenta bucatariei a fost inchisa mai devreme</t>
+  </si>
+  <si>
+    <t>Numele clasei OrdersGUI nu este sugestiv, un nume mai potrivit este TableGUI</t>
   </si>
 </sst>
 </file>
@@ -463,6 +466,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -505,9 +511,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,19 +876,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -898,7 +901,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>55</v>
       </c>
       <c r="J3" s="18">
@@ -909,14 +912,14 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="23" t="s">
         <v>56</v>
       </c>
       <c r="J4" s="3">
@@ -927,10 +930,10 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -942,15 +945,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -970,10 +973,10 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -985,7 +988,7 @@
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1172,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,19 +1196,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1218,7 +1221,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>55</v>
       </c>
       <c r="J3" s="18">
@@ -1229,14 +1232,14 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="23" t="s">
         <v>56</v>
       </c>
       <c r="J4" s="3">
@@ -1247,10 +1250,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1262,15 +1265,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1350,14 +1353,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
@@ -1491,7 +1498,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -1513,19 +1520,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1538,7 +1545,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>55</v>
       </c>
       <c r="J3" s="18">
@@ -1549,14 +1556,14 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="23" t="s">
         <v>56</v>
       </c>
       <c r="J4" s="3">
@@ -1567,10 +1574,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1582,15 +1589,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1879,19 +1886,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1911,8 +1918,8 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1923,8 +1930,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1936,8 +1943,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -2169,11 +2176,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check future isPresent before calling get()
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Documents\GitHub\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57921BCC-2942-43DD-99BA-BEF5C4199EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37384EC0-DECA-4D37-98F2-F090654ADCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -245,6 +245,20 @@
   </si>
   <si>
     <t>Numele clasei OrdersGUI nu este sugestiv, un nume mai potrivit este TableGUI</t>
+  </si>
+  <si>
+    <t>Main, 54, 62</t>
+  </si>
+  <si>
+    <t>Optional value should only be accessed after calling isPresent()</t>
+  </si>
+  <si>
+    <t>if (result.get() == ButtonType.YES){
+else if (result.get() == ButtonType.NO){</t>
+  </si>
+  <si>
+    <t>if (result.isPresent() &amp;&amp; result.get() == ButtonType.YES){
+else if (result.isPresent() &amp;&amp; result.get() == ButtonType.NO){</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1189,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1864,18 +1878,18 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="58.28515625" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1963,14 +1977,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">

</xml_diff>

<commit_message>
Replace anonymous inner class with lambda
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Documents\GitHub\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37384EC0-DECA-4D37-98F2-F090654ADCC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F87F4C-EE9B-434A-91B1-C8049AB45D3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -259,6 +259,18 @@
   <si>
     <t>if (result.isPresent() &amp;&amp; result.get() == ButtonType.YES){
 else if (result.isPresent() &amp;&amp; result.get() == ButtonType.NO){</t>
+  </si>
+  <si>
+    <t>primaryStage.setOnCloseRequest(new EventHandler&lt;WindowEvent&gt;() {</t>
+  </si>
+  <si>
+    <t>Main, 44</t>
+  </si>
+  <si>
+    <t>Anonymous inner classes containing only one method should become lambdas</t>
+  </si>
+  <si>
+    <t>primaryStage.setOnCloseRequest(event -&gt; {</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1891,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1899,7 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="37.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="58.28515625" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
@@ -1994,15 +2006,23 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">

</xml_diff>

<commit_message>
Remove empty String constructor
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Documents\GitHub\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F87F4C-EE9B-434A-91B1-C8049AB45D3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071BEDC-9673-4012-B439-72168AE5972B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>primaryStage.setOnCloseRequest(event -&gt; {</t>
+  </si>
+  <si>
+    <t>private String extractedTableNumberString = new String();</t>
+  </si>
+  <si>
+    <t>Constructors should not be used to instantiate "String", "BigInteger", "BigDecimal" and primitive-wrapper classes</t>
+  </si>
+  <si>
+    <t>KitchenGUIContorller, 28</t>
+  </si>
+  <si>
+    <t>private String extractedTableNumberString = "";</t>
   </si>
 </sst>
 </file>
@@ -1891,7 +1903,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,7 +1912,7 @@
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="46.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="58.28515625" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
@@ -2014,7 +2026,7 @@
       <c r="C11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2024,15 +2036,23 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">

</xml_diff>

<commit_message>
replaced size check with isEmpty method
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewBest\Documents\GitHub\Infinity16\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\An3Sem2\VVSS\git_inf_16\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071BEDC-9673-4012-B439-72168AE5972B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1AA931-7730-4C2D-9FFA-AD5E9D0E6008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -283,6 +294,18 @@
   </si>
   <si>
     <t>private String extractedTableNumberString = "";</t>
+  </si>
+  <si>
+    <t>PaymentsService, 26</t>
+  </si>
+  <si>
+    <t>if ((l==null) ||(l.size()==0)) return total;</t>
+  </si>
+  <si>
+    <t>Collection.isEmpty() should be used to test for emptiness</t>
+  </si>
+  <si>
+    <t>if (l==null || l.isEmpty()) return total;</t>
   </si>
 </sst>
 </file>
@@ -896,20 +919,20 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="6" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="6"/>
-    <col min="8" max="8" width="10.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="10.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="26.44140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -920,7 +943,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
@@ -935,7 +958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -946,7 +969,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -964,7 +987,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
@@ -978,7 +1001,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -986,14 +1009,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1007,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1021,7 +1044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1036,7 +1059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -1051,7 +1074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1066,7 +1089,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1081,7 +1104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1090,7 +1113,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1099,7 +1122,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1108,7 +1131,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1117,7 +1140,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1126,7 +1149,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1135,7 +1158,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1144,7 +1167,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1153,7 +1176,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1162,7 +1185,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1171,7 +1194,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1180,10 +1203,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1217,19 +1240,19 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" style="6" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="6"/>
-    <col min="8" max="8" width="10.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="10.88671875" style="6" customWidth="1"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1240,7 +1263,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
@@ -1255,7 +1278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1289,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1307,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1298,7 +1321,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1306,14 +1329,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1327,7 +1350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1339,7 +1362,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1352,7 +1375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1365,7 +1388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1378,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1391,7 +1414,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1404,7 +1427,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1413,7 +1436,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1422,7 +1445,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1431,7 +1454,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1440,7 +1463,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1449,7 +1472,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1458,7 +1481,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1467,7 +1490,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1476,7 +1499,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1485,7 +1508,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1494,7 +1517,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1503,10 +1526,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1540,20 +1563,20 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="55.140625" style="6" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="6"/>
-    <col min="8" max="8" width="11.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="55.109375" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="11.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1564,7 +1587,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
@@ -1579,7 +1602,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1590,7 +1613,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
@@ -1608,7 +1631,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
@@ -1622,7 +1645,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1630,14 +1653,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1651,7 +1674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1665,7 +1688,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1680,7 +1703,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1695,7 +1718,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1710,7 +1733,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1725,7 +1748,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1734,7 +1757,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1743,7 +1766,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1752,7 +1775,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1761,7 +1784,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1770,7 +1793,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1779,7 +1802,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1788,7 +1811,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1797,7 +1820,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1806,7 +1829,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1815,7 +1838,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1824,7 +1847,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1833,7 +1856,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1842,7 +1865,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1851,7 +1874,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1860,7 +1883,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1869,10 +1892,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -1902,24 +1925,24 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="58.28515625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="43.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1930,7 +1953,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
@@ -1945,14 +1968,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
@@ -1964,7 +1987,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1976,7 +1999,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1984,7 +2007,7 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2001,7 +2024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2018,7 +2041,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2036,7 +2059,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2054,17 +2077,25 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2074,7 +2105,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2084,7 +2115,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2094,7 +2125,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2104,7 +2135,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2114,7 +2145,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2124,7 +2155,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2134,7 +2165,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2144,7 +2175,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2154,7 +2185,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2164,7 +2195,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2174,7 +2205,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2184,7 +2215,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2194,7 +2225,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2204,7 +2235,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2214,7 +2245,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2224,7 +2255,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2234,10 +2265,10 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="36" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
removed duplicate code in PaymntAlert
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\An3Sem2\VVSS\git_inf_16\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1AA931-7730-4C2D-9FFA-AD5E9D0E6008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFE6C91-9798-46EF-B5B6-0FCF152C7027}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -306,6 +306,27 @@
   </si>
   <si>
     <t>if (l==null || l.isEmpty()) return total;</t>
+  </si>
+  <si>
+    <t>PaymentAlert, 55-61</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> } else if (result.get() == cancel) {
+             cancelPayment();
+             return false;
+        } else {
+            cancelPayment();
+            return false;
+        }</t>
+  </si>
+  <si>
+    <t>Two branches in a conditional structure should not have exactly the same implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   } else {
+            cancelPayment();
+            return false;
+        }</t>
   </si>
 </sst>
 </file>
@@ -1925,8 +1946,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2095,15 +2116,23 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">

</xml_diff>

<commit_message>
replaced annonymous inner class with lambda
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\An3Sem2\VVSS\git_inf_16\Infinity16\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFE6C91-9798-46EF-B5B6-0FCF152C7027}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D84EA4-739E-4E72-A7A7-945FFBD2C50A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -327,6 +327,15 @@
             cancelPayment();
             return false;
         }</t>
+  </si>
+  <si>
+    <t>KitchenGUI, 37</t>
+  </si>
+  <si>
+    <t>stage.setOnCloseRequest(new EventHandler&lt;WindowEvent&gt;() {</t>
+  </si>
+  <si>
+    <t>stage.setOnCloseRequest(event -&gt; {</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1956,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2134,15 +2143,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">

</xml_diff>